<commit_message>
organização final que foi enviada
</commit_message>
<xml_diff>
--- a/resultados_rede_neural.xlsx
+++ b/resultados_rede_neural.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CEFET-MG\IPB\Visão por Computador\trabalho-visao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E5EF9A-5654-4BCE-BE20-492A9FEFE13A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55649D7C-F72A-48A1-B0E1-4FD76C032597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="375" windowWidth="25440" windowHeight="15270" xr2:uid="{36AB984E-8AC5-4474-B9BF-681DFF9F62B8}"/>
+    <workbookView xWindow="28680" yWindow="375" windowWidth="25440" windowHeight="15270" xr2:uid="{D274F1FC-49E7-4B03-A878-71F6938F4879}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1356" uniqueCount="682">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1516" uniqueCount="762">
   <si>
     <t>Imagem</t>
   </si>
@@ -44,33 +44,234 @@
     <t>Resultado</t>
   </si>
   <si>
+    <t>0001_E_V_105_C.jpg</t>
+  </si>
+  <si>
+    <t>good_quality</t>
+  </si>
+  <si>
+    <t>0001_E_V_120_C.jpg</t>
+  </si>
+  <si>
+    <t>0001_E_V_135_C.jpg</t>
+  </si>
+  <si>
+    <t>0001_E_V_165_C.jpg</t>
+  </si>
+  <si>
+    <t>0001_E_V_90_D.jpg</t>
+  </si>
+  <si>
+    <t>bad_quality</t>
+  </si>
+  <si>
+    <t>0001_F_H_105_C.jpg</t>
+  </si>
+  <si>
+    <t>0001_F_H_120_C.jpg</t>
+  </si>
+  <si>
+    <t>0001_F_H_135_C.jpg</t>
+  </si>
+  <si>
+    <t>0001_F_H_150_C.jpg</t>
+  </si>
+  <si>
+    <t>0001_F_H_15_C.jpg</t>
+  </si>
+  <si>
+    <t>0001_F_H_165_C.jpg</t>
+  </si>
+  <si>
+    <t>0001_F_H_30_C.jpg</t>
+  </si>
+  <si>
+    <t>0001_F_H_45_C.jpg</t>
+  </si>
+  <si>
+    <t>0001_F_H_60_C.jpg</t>
+  </si>
+  <si>
+    <t>0001_F_H_75_C.jpg</t>
+  </si>
+  <si>
+    <t>0001_F_H_90_C.jpg</t>
+  </si>
+  <si>
+    <t>0001_F_I_0_C.jpg</t>
+  </si>
+  <si>
+    <t>0001_F_I_105_C.jpg</t>
+  </si>
+  <si>
+    <t>0001_F_I_120_C.jpg</t>
+  </si>
+  <si>
+    <t>0001_F_I_135_C.jpg</t>
+  </si>
+  <si>
+    <t>0001_F_I_150_C.jpg</t>
+  </si>
+  <si>
+    <t>0001_F_I_15_C.jpg</t>
+  </si>
+  <si>
+    <t>0001_F_I_165_C.jpg</t>
+  </si>
+  <si>
+    <t>0001_F_I_30_C.jpg</t>
+  </si>
+  <si>
+    <t>0001_F_I_45_C.jpg</t>
+  </si>
+  <si>
+    <t>0001_F_I_60_C.jpg</t>
+  </si>
+  <si>
+    <t>0001_F_I_75_C.jpg</t>
+  </si>
+  <si>
+    <t>0001_F_I_90_C.jpg</t>
+  </si>
+  <si>
     <t>0001_F_V_0_C.jpg</t>
   </si>
   <si>
-    <t>good_quality</t>
+    <t>0001_F_V_105_C.jpg</t>
+  </si>
+  <si>
+    <t>0001_F_V_120_C.jpg</t>
+  </si>
+  <si>
+    <t>0001_F_V_135_C.jpg</t>
+  </si>
+  <si>
+    <t>0001_F_V_150_C.jpg</t>
   </si>
   <si>
     <t>0001_F_V_15_C.jpg</t>
   </si>
   <si>
+    <t>0001_F_V_165_C.jpg</t>
+  </si>
+  <si>
     <t>0001_F_V_30_C.jpg</t>
   </si>
   <si>
+    <t>0001_F_V_45_C.jpg</t>
+  </si>
+  <si>
+    <t>0001_F_V_60_C.jpg</t>
+  </si>
+  <si>
     <t>0001_F_V_75_C.jpg</t>
   </si>
   <si>
     <t>0001_F_V_90_C.jpg</t>
   </si>
   <si>
+    <t>0001_G_H_0_A.jpg</t>
+  </si>
+  <si>
+    <t>0001_G_H_105_A.jpg</t>
+  </si>
+  <si>
+    <t>0001_G_H_120_A.jpg</t>
+  </si>
+  <si>
+    <t>0001_G_H_135_A.jpg</t>
+  </si>
+  <si>
+    <t>0001_G_H_150_A.jpg</t>
+  </si>
+  <si>
+    <t>0001_G_H_15_A.jpg</t>
+  </si>
+  <si>
+    <t>0001_G_H_165_A.jpg</t>
+  </si>
+  <si>
+    <t>0001_G_H_30_A.jpg</t>
+  </si>
+  <si>
+    <t>0001_G_H_45_A.jpg</t>
+  </si>
+  <si>
+    <t>0001_G_H_60_A.jpg</t>
+  </si>
+  <si>
+    <t>0001_G_H_75_A.jpg</t>
+  </si>
+  <si>
+    <t>0001_G_H_90_A.jpg</t>
+  </si>
+  <si>
+    <t>0001_G_I_0_A.jpg</t>
+  </si>
+  <si>
+    <t>0001_G_I_105_A.jpg</t>
+  </si>
+  <si>
+    <t>0001_G_I_120_A.jpg</t>
+  </si>
+  <si>
+    <t>0001_G_I_135_A.jpg</t>
+  </si>
+  <si>
     <t>0001_G_I_150_A.jpg</t>
   </si>
   <si>
-    <t>bad_quality</t>
+    <t>0001_G_I_15_A.jpg</t>
   </si>
   <si>
     <t>0001_G_I_165_A.jpg</t>
   </si>
   <si>
+    <t>0001_G_I_30_A.jpg</t>
+  </si>
+  <si>
+    <t>0001_G_I_45_A.jpg</t>
+  </si>
+  <si>
+    <t>0001_G_I_60_A.jpg</t>
+  </si>
+  <si>
+    <t>0001_G_I_75_A.jpg</t>
+  </si>
+  <si>
+    <t>0001_G_I_90_A.jpg</t>
+  </si>
+  <si>
+    <t>0001_G_V_0_A.jpg</t>
+  </si>
+  <si>
+    <t>0001_G_V_105_A.jpg</t>
+  </si>
+  <si>
+    <t>0001_G_V_120_A.jpg</t>
+  </si>
+  <si>
+    <t>0001_G_V_135_A.jpg</t>
+  </si>
+  <si>
+    <t>0001_G_V_15_A.jpg</t>
+  </si>
+  <si>
+    <t>0001_G_V_30_A.jpg</t>
+  </si>
+  <si>
+    <t>0001_G_V_45_A.jpg</t>
+  </si>
+  <si>
+    <t>0001_G_V_60_A.jpg</t>
+  </si>
+  <si>
+    <t>0001_G_V_75_A.jpg</t>
+  </si>
+  <si>
+    <t>0001_G_V_90_A.jpg</t>
+  </si>
+  <si>
     <t>0002_F_H_75_C.jpg</t>
   </si>
   <si>
@@ -1157,6 +1358,12 @@
     <t>bad_quality_292.jpg</t>
   </si>
   <si>
+    <t>bad_quality_36.jpg</t>
+  </si>
+  <si>
+    <t>bad_quality_37.jpg</t>
+  </si>
+  <si>
     <t>bad_quality_379.jpg</t>
   </si>
   <si>
@@ -1214,12 +1421,18 @@
     <t>bad_quality_62.jpg</t>
   </si>
   <si>
+    <t>bad_quality_63.jpg</t>
+  </si>
+  <si>
     <t>bad_quality_64.jpg</t>
   </si>
   <si>
     <t>bad_quality_644.jpg</t>
   </si>
   <si>
+    <t>bad_quality_65.jpg</t>
+  </si>
+  <si>
     <t>bad_quality_654.jpg</t>
   </si>
   <si>
@@ -1283,9 +1496,15 @@
     <t>bad_quality_858.jpg</t>
   </si>
   <si>
+    <t>bad_quality_86.jpg</t>
+  </si>
+  <si>
     <t>bad_quality_860.jpg</t>
   </si>
   <si>
+    <t>bad_quality_87.jpg</t>
+  </si>
+  <si>
     <t>bad_quality_882.jpg</t>
   </si>
   <si>
@@ -1295,6 +1514,9 @@
     <t>bad_quality_939.jpg</t>
   </si>
   <si>
+    <t>bad_quality_98.jpg</t>
+  </si>
+  <si>
     <t>empty_background_10.jpg</t>
   </si>
   <si>
@@ -1781,7 +2003,25 @@
     <t>good_quality_317.jpg</t>
   </si>
   <si>
+    <t>good_quality_32.jpg</t>
+  </si>
+  <si>
+    <t>good_quality_33.jpg</t>
+  </si>
+  <si>
     <t>good_quality_336.jpg</t>
+  </si>
+  <si>
+    <t>good_quality_34.jpg</t>
+  </si>
+  <si>
+    <t>good_quality_35.jpg</t>
+  </si>
+  <si>
+    <t>good_quality_36.jpg</t>
+  </si>
+  <si>
+    <t>good_quality_37.jpg</t>
   </si>
   <si>
     <t>good_quality_374.jpg</t>
@@ -2088,7 +2328,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2114,14 +2361,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2452,27 +2705,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C30340-19E1-443A-8414-E1AD4D5B97C9}">
-  <dimension ref="A1:B678"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC8AED10-6675-400C-8650-B90F242AD52C}">
+  <dimension ref="A1:H758"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="31.42578125" customWidth="1"/>
+    <col min="5" max="5" width="22" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2480,7 +2741,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2488,119 +2749,131 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
       <c r="B15" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
       <c r="B17" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -2608,7 +2881,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -2616,7 +2889,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -2624,7 +2897,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -2632,7 +2905,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -2640,7 +2913,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -2648,7 +2921,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -2656,7 +2929,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -2664,7 +2937,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -2672,7 +2945,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -2680,7 +2953,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -2688,7 +2961,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -2696,7 +2969,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -2704,7 +2977,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -2712,7 +2985,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -2797,7 +3070,7 @@
         <v>44</v>
       </c>
       <c r="B42" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2805,7 +3078,7 @@
         <v>45</v>
       </c>
       <c r="B43" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -2813,7 +3086,7 @@
         <v>46</v>
       </c>
       <c r="B44" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -2821,7 +3094,7 @@
         <v>47</v>
       </c>
       <c r="B45" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -2837,7 +3110,7 @@
         <v>49</v>
       </c>
       <c r="B47" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -2853,7 +3126,7 @@
         <v>51</v>
       </c>
       <c r="B49" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -2861,7 +3134,7 @@
         <v>52</v>
       </c>
       <c r="B50" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -2869,7 +3142,7 @@
         <v>53</v>
       </c>
       <c r="B51" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2877,7 +3150,7 @@
         <v>54</v>
       </c>
       <c r="B52" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -2885,7 +3158,7 @@
         <v>55</v>
       </c>
       <c r="B53" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -2917,7 +3190,7 @@
         <v>59</v>
       </c>
       <c r="B57" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -2925,7 +3198,7 @@
         <v>60</v>
       </c>
       <c r="B58" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -2941,7 +3214,7 @@
         <v>62</v>
       </c>
       <c r="B60" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -2997,7 +3270,7 @@
         <v>69</v>
       </c>
       <c r="B67" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -3005,7 +3278,7 @@
         <v>70</v>
       </c>
       <c r="B68" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -3013,7 +3286,7 @@
         <v>71</v>
       </c>
       <c r="B69" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -3101,7 +3374,7 @@
         <v>82</v>
       </c>
       <c r="B80" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -3109,7 +3382,7 @@
         <v>83</v>
       </c>
       <c r="B81" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -3381,7 +3654,7 @@
         <v>117</v>
       </c>
       <c r="B115" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
@@ -3389,7 +3662,7 @@
         <v>118</v>
       </c>
       <c r="B116" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
@@ -3397,7 +3670,7 @@
         <v>119</v>
       </c>
       <c r="B117" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
@@ -3557,7 +3830,7 @@
         <v>139</v>
       </c>
       <c r="B137" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
@@ -3565,7 +3838,7 @@
         <v>140</v>
       </c>
       <c r="B138" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
@@ -3917,7 +4190,7 @@
         <v>184</v>
       </c>
       <c r="B182" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
@@ -3925,7 +4198,7 @@
         <v>185</v>
       </c>
       <c r="B183" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
@@ -3933,7 +4206,7 @@
         <v>186</v>
       </c>
       <c r="B184" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
@@ -4093,7 +4366,7 @@
         <v>206</v>
       </c>
       <c r="B204" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
@@ -4101,7 +4374,7 @@
         <v>207</v>
       </c>
       <c r="B205" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
@@ -4277,7 +4550,7 @@
         <v>229</v>
       </c>
       <c r="B227" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
@@ -4285,7 +4558,7 @@
         <v>230</v>
       </c>
       <c r="B228" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
@@ -4293,7 +4566,7 @@
         <v>231</v>
       </c>
       <c r="B229" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
@@ -4301,7 +4574,7 @@
         <v>232</v>
       </c>
       <c r="B230" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
@@ -4309,7 +4582,7 @@
         <v>233</v>
       </c>
       <c r="B231" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
@@ -4317,7 +4590,7 @@
         <v>234</v>
       </c>
       <c r="B232" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
@@ -4485,7 +4758,7 @@
         <v>255</v>
       </c>
       <c r="B253" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
@@ -4501,7 +4774,7 @@
         <v>257</v>
       </c>
       <c r="B255" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
@@ -4813,7 +5086,7 @@
         <v>296</v>
       </c>
       <c r="B294" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
@@ -4821,7 +5094,7 @@
         <v>297</v>
       </c>
       <c r="B295" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.25">
@@ -4829,7 +5102,7 @@
         <v>298</v>
       </c>
       <c r="B296" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.25">
@@ -4837,7 +5110,7 @@
         <v>299</v>
       </c>
       <c r="B297" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
@@ -4845,7 +5118,7 @@
         <v>300</v>
       </c>
       <c r="B298" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
@@ -4853,7 +5126,7 @@
         <v>301</v>
       </c>
       <c r="B299" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
@@ -5021,7 +5294,7 @@
         <v>322</v>
       </c>
       <c r="B320" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.25">
@@ -5037,7 +5310,7 @@
         <v>324</v>
       </c>
       <c r="B322" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.25">
@@ -5229,7 +5502,7 @@
         <v>348</v>
       </c>
       <c r="B346" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.25">
@@ -5237,7 +5510,7 @@
         <v>349</v>
       </c>
       <c r="B347" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.25">
@@ -5245,7 +5518,7 @@
         <v>350</v>
       </c>
       <c r="B348" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.25">
@@ -5253,7 +5526,7 @@
         <v>351</v>
       </c>
       <c r="B349" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.25">
@@ -5261,7 +5534,7 @@
         <v>352</v>
       </c>
       <c r="B350" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.25">
@@ -5269,7 +5542,7 @@
         <v>353</v>
       </c>
       <c r="B351" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.25">
@@ -5277,7 +5550,7 @@
         <v>354</v>
       </c>
       <c r="B352" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.25">
@@ -5285,7 +5558,7 @@
         <v>355</v>
       </c>
       <c r="B353" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.25">
@@ -5293,7 +5566,7 @@
         <v>356</v>
       </c>
       <c r="B354" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.25">
@@ -5301,7 +5574,7 @@
         <v>357</v>
       </c>
       <c r="B355" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.25">
@@ -5309,7 +5582,7 @@
         <v>358</v>
       </c>
       <c r="B356" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.25">
@@ -5317,7 +5590,7 @@
         <v>359</v>
       </c>
       <c r="B357" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.25">
@@ -5325,7 +5598,7 @@
         <v>360</v>
       </c>
       <c r="B358" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.25">
@@ -5333,7 +5606,7 @@
         <v>361</v>
       </c>
       <c r="B359" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.25">
@@ -5341,7 +5614,7 @@
         <v>362</v>
       </c>
       <c r="B360" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.25">
@@ -5349,7 +5622,7 @@
         <v>363</v>
       </c>
       <c r="B361" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.25">
@@ -5357,7 +5630,7 @@
         <v>364</v>
       </c>
       <c r="B362" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.25">
@@ -5365,7 +5638,7 @@
         <v>365</v>
       </c>
       <c r="B363" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.25">
@@ -5373,7 +5646,7 @@
         <v>366</v>
       </c>
       <c r="B364" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.25">
@@ -5381,7 +5654,7 @@
         <v>367</v>
       </c>
       <c r="B365" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.25">
@@ -5389,7 +5662,7 @@
         <v>368</v>
       </c>
       <c r="B366" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.25">
@@ -5397,7 +5670,7 @@
         <v>369</v>
       </c>
       <c r="B367" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.25">
@@ -5405,7 +5678,7 @@
         <v>370</v>
       </c>
       <c r="B368" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.25">
@@ -5413,7 +5686,7 @@
         <v>371</v>
       </c>
       <c r="B369" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.25">
@@ -5421,7 +5694,7 @@
         <v>372</v>
       </c>
       <c r="B370" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.25">
@@ -5429,7 +5702,7 @@
         <v>373</v>
       </c>
       <c r="B371" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.25">
@@ -5437,7 +5710,7 @@
         <v>374</v>
       </c>
       <c r="B372" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.25">
@@ -5445,7 +5718,7 @@
         <v>375</v>
       </c>
       <c r="B373" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.25">
@@ -5453,7 +5726,7 @@
         <v>376</v>
       </c>
       <c r="B374" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.25">
@@ -5461,7 +5734,7 @@
         <v>377</v>
       </c>
       <c r="B375" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.25">
@@ -5469,7 +5742,7 @@
         <v>378</v>
       </c>
       <c r="B376" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.25">
@@ -5477,7 +5750,7 @@
         <v>379</v>
       </c>
       <c r="B377" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.25">
@@ -5485,7 +5758,7 @@
         <v>380</v>
       </c>
       <c r="B378" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.25">
@@ -5493,7 +5766,7 @@
         <v>381</v>
       </c>
       <c r="B379" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.25">
@@ -5501,7 +5774,7 @@
         <v>382</v>
       </c>
       <c r="B380" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.25">
@@ -5509,7 +5782,7 @@
         <v>383</v>
       </c>
       <c r="B381" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.25">
@@ -5517,7 +5790,7 @@
         <v>384</v>
       </c>
       <c r="B382" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.25">
@@ -5525,7 +5798,7 @@
         <v>385</v>
       </c>
       <c r="B383" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.25">
@@ -5533,7 +5806,7 @@
         <v>386</v>
       </c>
       <c r="B384" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.25">
@@ -5541,7 +5814,7 @@
         <v>387</v>
       </c>
       <c r="B385" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.25">
@@ -5549,7 +5822,7 @@
         <v>388</v>
       </c>
       <c r="B386" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.25">
@@ -5557,7 +5830,7 @@
         <v>389</v>
       </c>
       <c r="B387" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.25">
@@ -5565,7 +5838,7 @@
         <v>390</v>
       </c>
       <c r="B388" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.25">
@@ -5573,7 +5846,7 @@
         <v>391</v>
       </c>
       <c r="B389" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.25">
@@ -5581,7 +5854,7 @@
         <v>392</v>
       </c>
       <c r="B390" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.25">
@@ -5589,7 +5862,7 @@
         <v>393</v>
       </c>
       <c r="B391" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.25">
@@ -5597,7 +5870,7 @@
         <v>394</v>
       </c>
       <c r="B392" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.25">
@@ -5605,7 +5878,7 @@
         <v>395</v>
       </c>
       <c r="B393" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.25">
@@ -5613,7 +5886,7 @@
         <v>396</v>
       </c>
       <c r="B394" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.25">
@@ -5621,7 +5894,7 @@
         <v>397</v>
       </c>
       <c r="B395" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.25">
@@ -5629,7 +5902,7 @@
         <v>398</v>
       </c>
       <c r="B396" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.25">
@@ -5637,7 +5910,7 @@
         <v>399</v>
       </c>
       <c r="B397" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.25">
@@ -5645,7 +5918,7 @@
         <v>400</v>
       </c>
       <c r="B398" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.25">
@@ -5653,7 +5926,7 @@
         <v>401</v>
       </c>
       <c r="B399" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.25">
@@ -5661,7 +5934,7 @@
         <v>402</v>
       </c>
       <c r="B400" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.25">
@@ -5669,7 +5942,7 @@
         <v>403</v>
       </c>
       <c r="B401" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.25">
@@ -5677,7 +5950,7 @@
         <v>404</v>
       </c>
       <c r="B402" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.25">
@@ -5685,7 +5958,7 @@
         <v>405</v>
       </c>
       <c r="B403" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.25">
@@ -5693,7 +5966,7 @@
         <v>406</v>
       </c>
       <c r="B404" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.25">
@@ -5701,7 +5974,7 @@
         <v>407</v>
       </c>
       <c r="B405" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.25">
@@ -5709,7 +5982,7 @@
         <v>408</v>
       </c>
       <c r="B406" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.25">
@@ -5717,7 +5990,7 @@
         <v>409</v>
       </c>
       <c r="B407" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.25">
@@ -5725,7 +5998,7 @@
         <v>410</v>
       </c>
       <c r="B408" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.25">
@@ -5733,7 +6006,7 @@
         <v>411</v>
       </c>
       <c r="B409" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.25">
@@ -5741,7 +6014,7 @@
         <v>412</v>
       </c>
       <c r="B410" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.25">
@@ -5749,7 +6022,7 @@
         <v>413</v>
       </c>
       <c r="B411" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.25">
@@ -5757,7 +6030,7 @@
         <v>414</v>
       </c>
       <c r="B412" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.25">
@@ -5765,7 +6038,7 @@
         <v>415</v>
       </c>
       <c r="B413" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.25">
@@ -5773,7 +6046,7 @@
         <v>416</v>
       </c>
       <c r="B414" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.25">
@@ -5781,7 +6054,7 @@
         <v>417</v>
       </c>
       <c r="B415" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.25">
@@ -5789,7 +6062,7 @@
         <v>418</v>
       </c>
       <c r="B416" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.25">
@@ -5797,599 +6070,599 @@
         <v>419</v>
       </c>
       <c r="B417" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B418" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B419" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B420" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B421" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B422" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B423" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B424" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B425" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="426" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B426" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B427" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="428" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B428" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="429" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B429" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="430" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B430" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="431" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B431" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="432" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B432" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B433" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="434" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B434" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="435" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B435" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B436" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B437" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B438" t="s">
-        <v>420</v>
+        <v>3</v>
       </c>
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B439" t="s">
-        <v>420</v>
+        <v>3</v>
       </c>
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B440" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B441" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B442" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B443" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="444" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B444" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B445" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="446" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B446" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="447" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B447" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B448" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="449" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B449" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="450" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B450" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="451" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B451" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="452" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B452" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="453" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B453" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="454" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B454" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="455" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B455" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="456" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B456" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="457" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B457" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="458" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B458" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="459" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B459" t="s">
-        <v>420</v>
+        <v>3</v>
       </c>
     </row>
     <row r="460" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B460" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="461" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B461" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="462" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B462" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="463" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B463" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="464" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B464" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="465" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B465" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="466" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B466" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="467" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B467" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="468" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B468" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="469" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B469" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="470" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B470" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="471" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B471" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="472" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B472" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="473" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A473" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B473" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="474" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B474" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="475" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A475" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B475" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="476" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B476" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="477" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B477" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="478" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B478" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="479" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A479" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B479" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="480" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B480" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="481" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B481" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="482" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B482" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="483" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A483" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B483" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="484" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B484" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="485" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A485" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B485" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="486" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B486" t="s">
-        <v>420</v>
+        <v>3</v>
       </c>
     </row>
     <row r="487" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B487" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="488" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B488" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="489" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B489" t="s">
-        <v>420</v>
+        <v>8</v>
       </c>
     </row>
     <row r="490" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B490" t="s">
-        <v>420</v>
+        <v>3</v>
       </c>
     </row>
     <row r="491" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
+        <v>493</v>
+      </c>
+      <c r="B491" t="s">
         <v>494</v>
-      </c>
-      <c r="B491" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="492" spans="1:2" x14ac:dyDescent="0.25">
@@ -6397,7 +6670,7 @@
         <v>495</v>
       </c>
       <c r="B492" t="s">
-        <v>420</v>
+        <v>494</v>
       </c>
     </row>
     <row r="493" spans="1:2" x14ac:dyDescent="0.25">
@@ -6405,7 +6678,7 @@
         <v>496</v>
       </c>
       <c r="B493" t="s">
-        <v>420</v>
+        <v>494</v>
       </c>
     </row>
     <row r="494" spans="1:2" x14ac:dyDescent="0.25">
@@ -6413,7 +6686,7 @@
         <v>497</v>
       </c>
       <c r="B494" t="s">
-        <v>420</v>
+        <v>494</v>
       </c>
     </row>
     <row r="495" spans="1:2" x14ac:dyDescent="0.25">
@@ -6421,7 +6694,7 @@
         <v>498</v>
       </c>
       <c r="B495" t="s">
-        <v>420</v>
+        <v>494</v>
       </c>
     </row>
     <row r="496" spans="1:2" x14ac:dyDescent="0.25">
@@ -6429,7 +6702,7 @@
         <v>499</v>
       </c>
       <c r="B496" t="s">
-        <v>420</v>
+        <v>494</v>
       </c>
     </row>
     <row r="497" spans="1:2" x14ac:dyDescent="0.25">
@@ -6437,7 +6710,7 @@
         <v>500</v>
       </c>
       <c r="B497" t="s">
-        <v>420</v>
+        <v>494</v>
       </c>
     </row>
     <row r="498" spans="1:2" x14ac:dyDescent="0.25">
@@ -6445,7 +6718,7 @@
         <v>501</v>
       </c>
       <c r="B498" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="499" spans="1:2" x14ac:dyDescent="0.25">
@@ -6453,7 +6726,7 @@
         <v>502</v>
       </c>
       <c r="B499" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="500" spans="1:2" x14ac:dyDescent="0.25">
@@ -6461,7 +6734,7 @@
         <v>503</v>
       </c>
       <c r="B500" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="501" spans="1:2" x14ac:dyDescent="0.25">
@@ -6469,7 +6742,7 @@
         <v>504</v>
       </c>
       <c r="B501" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="502" spans="1:2" x14ac:dyDescent="0.25">
@@ -6477,7 +6750,7 @@
         <v>505</v>
       </c>
       <c r="B502" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="503" spans="1:2" x14ac:dyDescent="0.25">
@@ -6485,7 +6758,7 @@
         <v>506</v>
       </c>
       <c r="B503" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="504" spans="1:2" x14ac:dyDescent="0.25">
@@ -6493,7 +6766,7 @@
         <v>507</v>
       </c>
       <c r="B504" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="505" spans="1:2" x14ac:dyDescent="0.25">
@@ -6501,7 +6774,7 @@
         <v>508</v>
       </c>
       <c r="B505" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="506" spans="1:2" x14ac:dyDescent="0.25">
@@ -6509,7 +6782,7 @@
         <v>509</v>
       </c>
       <c r="B506" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="507" spans="1:2" x14ac:dyDescent="0.25">
@@ -6517,7 +6790,7 @@
         <v>510</v>
       </c>
       <c r="B507" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="508" spans="1:2" x14ac:dyDescent="0.25">
@@ -6525,7 +6798,7 @@
         <v>511</v>
       </c>
       <c r="B508" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="509" spans="1:2" x14ac:dyDescent="0.25">
@@ -6533,7 +6806,7 @@
         <v>512</v>
       </c>
       <c r="B509" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="510" spans="1:2" x14ac:dyDescent="0.25">
@@ -6541,7 +6814,7 @@
         <v>513</v>
       </c>
       <c r="B510" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="511" spans="1:2" x14ac:dyDescent="0.25">
@@ -6549,7 +6822,7 @@
         <v>514</v>
       </c>
       <c r="B511" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="512" spans="1:2" x14ac:dyDescent="0.25">
@@ -6557,7 +6830,7 @@
         <v>515</v>
       </c>
       <c r="B512" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="513" spans="1:2" x14ac:dyDescent="0.25">
@@ -6565,7 +6838,7 @@
         <v>516</v>
       </c>
       <c r="B513" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="514" spans="1:2" x14ac:dyDescent="0.25">
@@ -6573,7 +6846,7 @@
         <v>517</v>
       </c>
       <c r="B514" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="515" spans="1:2" x14ac:dyDescent="0.25">
@@ -6581,7 +6854,7 @@
         <v>518</v>
       </c>
       <c r="B515" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="516" spans="1:2" x14ac:dyDescent="0.25">
@@ -6589,7 +6862,7 @@
         <v>519</v>
       </c>
       <c r="B516" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="517" spans="1:2" x14ac:dyDescent="0.25">
@@ -6597,7 +6870,7 @@
         <v>520</v>
       </c>
       <c r="B517" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="518" spans="1:2" x14ac:dyDescent="0.25">
@@ -6605,7 +6878,7 @@
         <v>521</v>
       </c>
       <c r="B518" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="519" spans="1:2" x14ac:dyDescent="0.25">
@@ -6613,7 +6886,7 @@
         <v>522</v>
       </c>
       <c r="B519" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="520" spans="1:2" x14ac:dyDescent="0.25">
@@ -6621,7 +6894,7 @@
         <v>523</v>
       </c>
       <c r="B520" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="521" spans="1:2" x14ac:dyDescent="0.25">
@@ -6629,7 +6902,7 @@
         <v>524</v>
       </c>
       <c r="B521" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="522" spans="1:2" x14ac:dyDescent="0.25">
@@ -6637,7 +6910,7 @@
         <v>525</v>
       </c>
       <c r="B522" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="523" spans="1:2" x14ac:dyDescent="0.25">
@@ -6645,7 +6918,7 @@
         <v>526</v>
       </c>
       <c r="B523" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="524" spans="1:2" x14ac:dyDescent="0.25">
@@ -6653,7 +6926,7 @@
         <v>527</v>
       </c>
       <c r="B524" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="525" spans="1:2" x14ac:dyDescent="0.25">
@@ -6661,7 +6934,7 @@
         <v>528</v>
       </c>
       <c r="B525" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="526" spans="1:2" x14ac:dyDescent="0.25">
@@ -6669,7 +6942,7 @@
         <v>529</v>
       </c>
       <c r="B526" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="527" spans="1:2" x14ac:dyDescent="0.25">
@@ -6677,7 +6950,7 @@
         <v>530</v>
       </c>
       <c r="B527" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="528" spans="1:2" x14ac:dyDescent="0.25">
@@ -6685,7 +6958,7 @@
         <v>531</v>
       </c>
       <c r="B528" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="529" spans="1:2" x14ac:dyDescent="0.25">
@@ -6693,7 +6966,7 @@
         <v>532</v>
       </c>
       <c r="B529" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="530" spans="1:2" x14ac:dyDescent="0.25">
@@ -6701,7 +6974,7 @@
         <v>533</v>
       </c>
       <c r="B530" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="531" spans="1:2" x14ac:dyDescent="0.25">
@@ -6709,7 +6982,7 @@
         <v>534</v>
       </c>
       <c r="B531" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="532" spans="1:2" x14ac:dyDescent="0.25">
@@ -6717,7 +6990,7 @@
         <v>535</v>
       </c>
       <c r="B532" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="533" spans="1:2" x14ac:dyDescent="0.25">
@@ -6725,7 +6998,7 @@
         <v>536</v>
       </c>
       <c r="B533" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="534" spans="1:2" x14ac:dyDescent="0.25">
@@ -6733,7 +7006,7 @@
         <v>537</v>
       </c>
       <c r="B534" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="535" spans="1:2" x14ac:dyDescent="0.25">
@@ -6741,7 +7014,7 @@
         <v>538</v>
       </c>
       <c r="B535" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="536" spans="1:2" x14ac:dyDescent="0.25">
@@ -6749,7 +7022,7 @@
         <v>539</v>
       </c>
       <c r="B536" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="537" spans="1:2" x14ac:dyDescent="0.25">
@@ -6757,7 +7030,7 @@
         <v>540</v>
       </c>
       <c r="B537" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="538" spans="1:2" x14ac:dyDescent="0.25">
@@ -6765,7 +7038,7 @@
         <v>541</v>
       </c>
       <c r="B538" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="539" spans="1:2" x14ac:dyDescent="0.25">
@@ -6773,7 +7046,7 @@
         <v>542</v>
       </c>
       <c r="B539" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="540" spans="1:2" x14ac:dyDescent="0.25">
@@ -6781,7 +7054,7 @@
         <v>543</v>
       </c>
       <c r="B540" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="541" spans="1:2" x14ac:dyDescent="0.25">
@@ -6789,7 +7062,7 @@
         <v>544</v>
       </c>
       <c r="B541" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="542" spans="1:2" x14ac:dyDescent="0.25">
@@ -6797,7 +7070,7 @@
         <v>545</v>
       </c>
       <c r="B542" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="543" spans="1:2" x14ac:dyDescent="0.25">
@@ -6805,7 +7078,7 @@
         <v>546</v>
       </c>
       <c r="B543" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="544" spans="1:2" x14ac:dyDescent="0.25">
@@ -6813,7 +7086,7 @@
         <v>547</v>
       </c>
       <c r="B544" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="545" spans="1:2" x14ac:dyDescent="0.25">
@@ -6821,7 +7094,7 @@
         <v>548</v>
       </c>
       <c r="B545" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="546" spans="1:2" x14ac:dyDescent="0.25">
@@ -6829,7 +7102,7 @@
         <v>549</v>
       </c>
       <c r="B546" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="547" spans="1:2" x14ac:dyDescent="0.25">
@@ -6837,7 +7110,7 @@
         <v>550</v>
       </c>
       <c r="B547" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="548" spans="1:2" x14ac:dyDescent="0.25">
@@ -6845,7 +7118,7 @@
         <v>551</v>
       </c>
       <c r="B548" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="549" spans="1:2" x14ac:dyDescent="0.25">
@@ -6853,7 +7126,7 @@
         <v>552</v>
       </c>
       <c r="B549" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="550" spans="1:2" x14ac:dyDescent="0.25">
@@ -6861,7 +7134,7 @@
         <v>553</v>
       </c>
       <c r="B550" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="551" spans="1:2" x14ac:dyDescent="0.25">
@@ -6869,7 +7142,7 @@
         <v>554</v>
       </c>
       <c r="B551" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="552" spans="1:2" x14ac:dyDescent="0.25">
@@ -6877,7 +7150,7 @@
         <v>555</v>
       </c>
       <c r="B552" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="553" spans="1:2" x14ac:dyDescent="0.25">
@@ -6885,7 +7158,7 @@
         <v>556</v>
       </c>
       <c r="B553" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="554" spans="1:2" x14ac:dyDescent="0.25">
@@ -6893,7 +7166,7 @@
         <v>557</v>
       </c>
       <c r="B554" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="555" spans="1:2" x14ac:dyDescent="0.25">
@@ -6901,7 +7174,7 @@
         <v>558</v>
       </c>
       <c r="B555" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="556" spans="1:2" x14ac:dyDescent="0.25">
@@ -6909,7 +7182,7 @@
         <v>559</v>
       </c>
       <c r="B556" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="557" spans="1:2" x14ac:dyDescent="0.25">
@@ -6917,7 +7190,7 @@
         <v>560</v>
       </c>
       <c r="B557" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="558" spans="1:2" x14ac:dyDescent="0.25">
@@ -6925,7 +7198,7 @@
         <v>561</v>
       </c>
       <c r="B558" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="559" spans="1:2" x14ac:dyDescent="0.25">
@@ -6933,7 +7206,7 @@
         <v>562</v>
       </c>
       <c r="B559" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="560" spans="1:2" x14ac:dyDescent="0.25">
@@ -6941,7 +7214,7 @@
         <v>563</v>
       </c>
       <c r="B560" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="561" spans="1:2" x14ac:dyDescent="0.25">
@@ -6949,7 +7222,7 @@
         <v>564</v>
       </c>
       <c r="B561" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="562" spans="1:2" x14ac:dyDescent="0.25">
@@ -6957,7 +7230,7 @@
         <v>565</v>
       </c>
       <c r="B562" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="563" spans="1:2" x14ac:dyDescent="0.25">
@@ -6965,7 +7238,7 @@
         <v>566</v>
       </c>
       <c r="B563" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="564" spans="1:2" x14ac:dyDescent="0.25">
@@ -6973,7 +7246,7 @@
         <v>567</v>
       </c>
       <c r="B564" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="565" spans="1:2" x14ac:dyDescent="0.25">
@@ -6981,7 +7254,7 @@
         <v>568</v>
       </c>
       <c r="B565" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="566" spans="1:2" x14ac:dyDescent="0.25">
@@ -6989,7 +7262,7 @@
         <v>569</v>
       </c>
       <c r="B566" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="567" spans="1:2" x14ac:dyDescent="0.25">
@@ -6997,7 +7270,7 @@
         <v>570</v>
       </c>
       <c r="B567" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="568" spans="1:2" x14ac:dyDescent="0.25">
@@ -7005,7 +7278,7 @@
         <v>571</v>
       </c>
       <c r="B568" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="569" spans="1:2" x14ac:dyDescent="0.25">
@@ -7013,7 +7286,7 @@
         <v>572</v>
       </c>
       <c r="B569" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="570" spans="1:2" x14ac:dyDescent="0.25">
@@ -7021,7 +7294,7 @@
         <v>573</v>
       </c>
       <c r="B570" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="571" spans="1:2" x14ac:dyDescent="0.25">
@@ -7029,7 +7302,7 @@
         <v>574</v>
       </c>
       <c r="B571" t="s">
-        <v>3</v>
+        <v>494</v>
       </c>
     </row>
     <row r="572" spans="1:2" x14ac:dyDescent="0.25">
@@ -7885,6 +8158,646 @@
         <v>681</v>
       </c>
       <c r="B678" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="679" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A679" t="s">
+        <v>682</v>
+      </c>
+      <c r="B679" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="680" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A680" t="s">
+        <v>683</v>
+      </c>
+      <c r="B680" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="681" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A681" t="s">
+        <v>684</v>
+      </c>
+      <c r="B681" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="682" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A682" t="s">
+        <v>685</v>
+      </c>
+      <c r="B682" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="683" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A683" t="s">
+        <v>686</v>
+      </c>
+      <c r="B683" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="684" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A684" t="s">
+        <v>687</v>
+      </c>
+      <c r="B684" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="685" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A685" t="s">
+        <v>688</v>
+      </c>
+      <c r="B685" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="686" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A686" t="s">
+        <v>689</v>
+      </c>
+      <c r="B686" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="687" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A687" t="s">
+        <v>690</v>
+      </c>
+      <c r="B687" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="688" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A688" t="s">
+        <v>691</v>
+      </c>
+      <c r="B688" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="689" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A689" t="s">
+        <v>692</v>
+      </c>
+      <c r="B689" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="690" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A690" t="s">
+        <v>693</v>
+      </c>
+      <c r="B690" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="691" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A691" t="s">
+        <v>694</v>
+      </c>
+      <c r="B691" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="692" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A692" t="s">
+        <v>695</v>
+      </c>
+      <c r="B692" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="693" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A693" t="s">
+        <v>696</v>
+      </c>
+      <c r="B693" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="694" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A694" t="s">
+        <v>697</v>
+      </c>
+      <c r="B694" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="695" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A695" t="s">
+        <v>698</v>
+      </c>
+      <c r="B695" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="696" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A696" t="s">
+        <v>699</v>
+      </c>
+      <c r="B696" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="697" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A697" t="s">
+        <v>700</v>
+      </c>
+      <c r="B697" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="698" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A698" t="s">
+        <v>701</v>
+      </c>
+      <c r="B698" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="699" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A699" t="s">
+        <v>702</v>
+      </c>
+      <c r="B699" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="700" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A700" t="s">
+        <v>703</v>
+      </c>
+      <c r="B700" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="701" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A701" t="s">
+        <v>704</v>
+      </c>
+      <c r="B701" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="702" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A702" t="s">
+        <v>705</v>
+      </c>
+      <c r="B702" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="703" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A703" t="s">
+        <v>706</v>
+      </c>
+      <c r="B703" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="704" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A704" t="s">
+        <v>707</v>
+      </c>
+      <c r="B704" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="705" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A705" t="s">
+        <v>708</v>
+      </c>
+      <c r="B705" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="706" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A706" t="s">
+        <v>709</v>
+      </c>
+      <c r="B706" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="707" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A707" t="s">
+        <v>710</v>
+      </c>
+      <c r="B707" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="708" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A708" t="s">
+        <v>711</v>
+      </c>
+      <c r="B708" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="709" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A709" t="s">
+        <v>712</v>
+      </c>
+      <c r="B709" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="710" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A710" t="s">
+        <v>713</v>
+      </c>
+      <c r="B710" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="711" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A711" t="s">
+        <v>714</v>
+      </c>
+      <c r="B711" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="712" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A712" t="s">
+        <v>715</v>
+      </c>
+      <c r="B712" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="713" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A713" t="s">
+        <v>716</v>
+      </c>
+      <c r="B713" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="714" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A714" t="s">
+        <v>717</v>
+      </c>
+      <c r="B714" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="715" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A715" t="s">
+        <v>718</v>
+      </c>
+      <c r="B715" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="716" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A716" t="s">
+        <v>719</v>
+      </c>
+      <c r="B716" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="717" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A717" t="s">
+        <v>720</v>
+      </c>
+      <c r="B717" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="718" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A718" t="s">
+        <v>721</v>
+      </c>
+      <c r="B718" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="719" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A719" t="s">
+        <v>722</v>
+      </c>
+      <c r="B719" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="720" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A720" t="s">
+        <v>723</v>
+      </c>
+      <c r="B720" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="721" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A721" t="s">
+        <v>724</v>
+      </c>
+      <c r="B721" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="722" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A722" t="s">
+        <v>725</v>
+      </c>
+      <c r="B722" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="723" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A723" t="s">
+        <v>726</v>
+      </c>
+      <c r="B723" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="724" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A724" t="s">
+        <v>727</v>
+      </c>
+      <c r="B724" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="725" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A725" t="s">
+        <v>728</v>
+      </c>
+      <c r="B725" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="726" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A726" t="s">
+        <v>729</v>
+      </c>
+      <c r="B726" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="727" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A727" t="s">
+        <v>730</v>
+      </c>
+      <c r="B727" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="728" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A728" t="s">
+        <v>731</v>
+      </c>
+      <c r="B728" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="729" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A729" t="s">
+        <v>732</v>
+      </c>
+      <c r="B729" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="730" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A730" t="s">
+        <v>733</v>
+      </c>
+      <c r="B730" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="731" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A731" t="s">
+        <v>734</v>
+      </c>
+      <c r="B731" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="732" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A732" t="s">
+        <v>735</v>
+      </c>
+      <c r="B732" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="733" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A733" t="s">
+        <v>736</v>
+      </c>
+      <c r="B733" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="734" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A734" t="s">
+        <v>737</v>
+      </c>
+      <c r="B734" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="735" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A735" t="s">
+        <v>738</v>
+      </c>
+      <c r="B735" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="736" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A736" t="s">
+        <v>739</v>
+      </c>
+      <c r="B736" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="737" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A737" t="s">
+        <v>740</v>
+      </c>
+      <c r="B737" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="738" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A738" t="s">
+        <v>741</v>
+      </c>
+      <c r="B738" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="739" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A739" t="s">
+        <v>742</v>
+      </c>
+      <c r="B739" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="740" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A740" t="s">
+        <v>743</v>
+      </c>
+      <c r="B740" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="741" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A741" t="s">
+        <v>744</v>
+      </c>
+      <c r="B741" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="742" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A742" t="s">
+        <v>745</v>
+      </c>
+      <c r="B742" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="743" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A743" t="s">
+        <v>746</v>
+      </c>
+      <c r="B743" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="744" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A744" t="s">
+        <v>747</v>
+      </c>
+      <c r="B744" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="745" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A745" t="s">
+        <v>748</v>
+      </c>
+      <c r="B745" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="746" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A746" t="s">
+        <v>749</v>
+      </c>
+      <c r="B746" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="747" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A747" t="s">
+        <v>750</v>
+      </c>
+      <c r="B747" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="748" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A748" t="s">
+        <v>751</v>
+      </c>
+      <c r="B748" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="749" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A749" t="s">
+        <v>752</v>
+      </c>
+      <c r="B749" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="750" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A750" t="s">
+        <v>753</v>
+      </c>
+      <c r="B750" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="751" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A751" t="s">
+        <v>754</v>
+      </c>
+      <c r="B751" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="752" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A752" t="s">
+        <v>755</v>
+      </c>
+      <c r="B752" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="753" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A753" t="s">
+        <v>756</v>
+      </c>
+      <c r="B753" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="754" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A754" t="s">
+        <v>757</v>
+      </c>
+      <c r="B754" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="755" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A755" t="s">
+        <v>758</v>
+      </c>
+      <c r="B755" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="756" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A756" t="s">
+        <v>759</v>
+      </c>
+      <c r="B756" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="757" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A757" t="s">
+        <v>760</v>
+      </c>
+      <c r="B757" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="758" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A758" t="s">
+        <v>761</v>
+      </c>
+      <c r="B758" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>